<commit_message>
fix bugs and rename fields in xlsx
</commit_message>
<xml_diff>
--- a/重庆多条件组合查询-代码生成配置.xlsx
+++ b/重庆多条件组合查询-代码生成配置.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="182">
   <si>
     <t>个性指标分类</t>
   </si>
@@ -339,16 +339,25 @@
     <t>[0-40],(40-80],(80-120],(120-160],(160-200]，200以上</t>
   </si>
   <si>
+    <t>arpu</t>
+  </si>
+  <si>
     <t>MOU</t>
   </si>
   <si>
     <t>[0-30],(30-200],(200-300],(300-500],(500-800],800以上</t>
   </si>
   <si>
+    <t>mou</t>
+  </si>
+  <si>
     <t>DOU</t>
   </si>
   <si>
     <t>[0-1]，(1-10]，(10-30]，(30-40]，(40-50]，50以上</t>
+  </si>
+  <si>
+    <t>dou</t>
   </si>
   <si>
     <t>是否办理不限量叠加包</t>
@@ -590,10 +599,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -619,7 +628,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -641,23 +650,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -680,6 +681,51 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -689,17 +735,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -713,43 +759,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,19 +790,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -811,7 +856,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,13 +886,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,19 +928,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -865,67 +946,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,31 +964,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1030,11 +1039,65 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1056,45 +1119,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1103,166 +1127,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1625,8 +1634,8 @@
   <sheetPr/>
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72072072072072" defaultRowHeight="13.5"/>
@@ -2839,10 +2848,10 @@
         <v>18</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
@@ -2860,13 +2869,13 @@
     <row r="32" spans="1:12">
       <c r="A32" s="3"/>
       <c r="B32" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>24</v>
@@ -2878,10 +2887,10 @@
         <v>18</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
@@ -2899,13 +2908,13 @@
     <row r="33" spans="1:12">
       <c r="A33" s="3"/>
       <c r="B33" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>24</v>
@@ -2917,10 +2926,10 @@
         <v>18</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
@@ -2938,7 +2947,7 @@
     <row r="34" spans="1:12">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>33</v>
@@ -2956,10 +2965,10 @@
         <v>18</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
@@ -2977,7 +2986,7 @@
     <row r="35" spans="1:12">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>33</v>
@@ -2995,10 +3004,10 @@
         <v>18</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
@@ -3015,16 +3024,16 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>24</v>
@@ -3036,10 +3045,10 @@
         <v>18</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
@@ -3057,13 +3066,13 @@
     <row r="37" spans="1:12">
       <c r="A37" s="8"/>
       <c r="B37" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>24</v>
@@ -3075,10 +3084,10 @@
         <v>18</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
@@ -3096,13 +3105,13 @@
     <row r="38" spans="1:12">
       <c r="A38" s="8"/>
       <c r="B38" s="6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>24</v>
@@ -3114,10 +3123,10 @@
         <v>18</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
@@ -3135,13 +3144,13 @@
     <row r="39" spans="1:12">
       <c r="A39" s="8"/>
       <c r="B39" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>24</v>
@@ -3153,10 +3162,10 @@
         <v>18</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
@@ -3174,13 +3183,13 @@
     <row r="40" spans="1:12">
       <c r="A40" s="8"/>
       <c r="B40" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>24</v>
@@ -3192,10 +3201,10 @@
         <v>18</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
@@ -3213,13 +3222,13 @@
     <row r="41" spans="1:12">
       <c r="A41" s="8"/>
       <c r="B41" s="6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>24</v>
@@ -3231,10 +3240,10 @@
         <v>18</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
@@ -3252,7 +3261,7 @@
     <row r="42" spans="1:12">
       <c r="A42" s="8"/>
       <c r="B42" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>33</v>
@@ -3270,10 +3279,10 @@
         <v>18</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
@@ -3291,13 +3300,13 @@
     <row r="43" spans="1:12">
       <c r="A43" s="8"/>
       <c r="B43" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>24</v>
@@ -3309,10 +3318,10 @@
         <v>18</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
@@ -3330,13 +3339,13 @@
     <row r="44" spans="1:12">
       <c r="A44" s="8"/>
       <c r="B44" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>24</v>
@@ -3348,10 +3357,10 @@
         <v>18</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
@@ -3369,13 +3378,13 @@
     <row r="45" spans="1:12">
       <c r="A45" s="8"/>
       <c r="B45" s="4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>24</v>
@@ -3387,10 +3396,10 @@
         <v>18</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
@@ -3408,13 +3417,13 @@
     <row r="46" spans="1:12">
       <c r="A46" s="8"/>
       <c r="B46" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>24</v>
@@ -3426,10 +3435,10 @@
         <v>18</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
@@ -3447,13 +3456,13 @@
     <row r="47" spans="1:12">
       <c r="A47" s="8"/>
       <c r="B47" s="4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>24</v>
@@ -3465,10 +3474,10 @@
         <v>18</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
@@ -3486,13 +3495,13 @@
     <row r="48" spans="1:12">
       <c r="A48" s="8"/>
       <c r="B48" s="4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>24</v>
@@ -3504,10 +3513,10 @@
         <v>18</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
@@ -3525,13 +3534,13 @@
     <row r="49" spans="1:12">
       <c r="A49" s="8"/>
       <c r="B49" s="4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>24</v>
@@ -3543,10 +3552,10 @@
         <v>18</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
@@ -3564,13 +3573,13 @@
     <row r="50" spans="1:12">
       <c r="A50" s="8"/>
       <c r="B50" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>24</v>
@@ -3582,10 +3591,10 @@
         <v>18</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
@@ -3603,13 +3612,13 @@
     <row r="51" spans="1:12">
       <c r="A51" s="8"/>
       <c r="B51" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>24</v>
@@ -3621,10 +3630,10 @@
         <v>18</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
@@ -3642,13 +3651,13 @@
     <row r="52" spans="1:12">
       <c r="A52" s="8"/>
       <c r="B52" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>24</v>
@@ -3660,10 +3669,10 @@
         <v>18</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
@@ -3681,13 +3690,13 @@
     <row r="53" spans="1:12">
       <c r="A53" s="8"/>
       <c r="B53" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>24</v>
@@ -3699,10 +3708,10 @@
         <v>18</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
@@ -3720,13 +3729,13 @@
     <row r="54" spans="1:12">
       <c r="A54" s="8"/>
       <c r="B54" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>24</v>
@@ -3738,10 +3747,10 @@
         <v>18</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
@@ -3759,13 +3768,13 @@
     <row r="55" spans="1:12">
       <c r="A55" s="8"/>
       <c r="B55" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>24</v>
@@ -3777,10 +3786,10 @@
         <v>18</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
@@ -3798,13 +3807,13 @@
     <row r="56" spans="1:12">
       <c r="A56" s="8"/>
       <c r="B56" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>24</v>
@@ -3816,10 +3825,10 @@
         <v>18</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
@@ -3837,13 +3846,13 @@
     <row r="57" spans="1:12">
       <c r="A57" s="8"/>
       <c r="B57" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>24</v>
@@ -3855,10 +3864,10 @@
         <v>18</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
@@ -3876,13 +3885,13 @@
     <row r="58" spans="1:12">
       <c r="A58" s="8"/>
       <c r="B58" s="6" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>24</v>
@@ -3894,10 +3903,10 @@
         <v>18</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
@@ -3915,13 +3924,13 @@
     <row r="59" spans="1:12">
       <c r="A59" s="8"/>
       <c r="B59" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>24</v>
@@ -3933,10 +3942,10 @@
         <v>18</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
@@ -3954,13 +3963,13 @@
     <row r="60" spans="1:12">
       <c r="A60" s="8"/>
       <c r="B60" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>24</v>
@@ -3972,10 +3981,10 @@
         <v>18</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
@@ -3993,13 +4002,13 @@
     <row r="61" spans="1:12">
       <c r="A61" s="8"/>
       <c r="B61" s="6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>24</v>
@@ -4011,10 +4020,10 @@
         <v>18</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
@@ -4032,13 +4041,13 @@
     <row r="62" spans="1:12">
       <c r="A62" s="8"/>
       <c r="B62" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>24</v>
@@ -4050,10 +4059,10 @@
         <v>18</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
@@ -4071,13 +4080,13 @@
     <row r="63" spans="1:12">
       <c r="A63" s="9"/>
       <c r="B63" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>24</v>
@@ -4089,10 +4098,10 @@
         <v>18</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
@@ -4109,16 +4118,16 @@
     </row>
     <row r="64" ht="13.6" spans="1:12">
       <c r="A64" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>16</v>
@@ -4130,10 +4139,10 @@
         <v>18</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>

</xml_diff>